<commit_message>
Fix issue w/ new capital project EIB template
</commit_message>
<xml_diff>
--- a/files/COB New Capital Project Budget EIB Load Template.xlsx
+++ b/files/COB New Capital Project Budget EIB Load Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elipousson/Projects/00_dop/baltimoreCIP-Workday-EIB/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D571B0D-EF21-C340-B255-82B8C1D754EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF5F74A-D502-5141-9C34-3C5BA2068C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="640" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import Budget High Volume" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Budget Lines Data'!$A$5:$W$396</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Import Budget High Volume'!$A$5:$K$147</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>Import Budget High Volume</t>
   </si>
@@ -200,97 +200,7 @@
     <t>Revenue Category</t>
   </si>
   <si>
-    <t>Jul</t>
-  </si>
-  <si>
-    <t>9936</t>
-  </si>
-  <si>
-    <t>CAP009457</t>
-  </si>
-  <si>
-    <t>9910</t>
-  </si>
-  <si>
-    <t>9916</t>
-  </si>
-  <si>
-    <t>RES009194</t>
-  </si>
-  <si>
-    <t>RES009600</t>
-  </si>
-  <si>
-    <t>9953</t>
-  </si>
-  <si>
-    <t>CAP009534</t>
-  </si>
-  <si>
-    <t>CAP009197</t>
-  </si>
-  <si>
-    <t>CAP009601</t>
-  </si>
-  <si>
-    <t>AllProjectBudgetRevenues</t>
-  </si>
-  <si>
-    <t>Parent_Account_Set</t>
-  </si>
-  <si>
-    <t>RC0650</t>
-  </si>
-  <si>
-    <t>AllBudgetExpenses</t>
-  </si>
-  <si>
-    <t>RC0605</t>
-  </si>
-  <si>
-    <t>RC0603</t>
-  </si>
-  <si>
-    <t>RC0651</t>
-  </si>
-  <si>
     <t>Ledger_Account_Summary_ID</t>
-  </si>
-  <si>
-    <t>PRJ002615</t>
-  </si>
-  <si>
-    <t>PRJ002672</t>
-  </si>
-  <si>
-    <t>PRJ002673</t>
-  </si>
-  <si>
-    <t>PRJ002477</t>
-  </si>
-  <si>
-    <t>PRJ002476</t>
-  </si>
-  <si>
-    <t>PRJ002675</t>
-  </si>
-  <si>
-    <t>PRJ002471</t>
-  </si>
-  <si>
-    <t>PRJ002554</t>
-  </si>
-  <si>
-    <t>PRJ002674</t>
-  </si>
-  <si>
-    <t>PRJ002339</t>
-  </si>
-  <si>
-    <t>PRJ002016</t>
-  </si>
-  <si>
-    <t>FY-23 Capital Budget</t>
   </si>
 </sst>
 </file>
@@ -452,7 +362,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,18 +564,6 @@
       <patternFill patternType="lightGrid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -881,15 +779,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1253,11 +1148,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="I173" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6:J188"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1274,40 +1169,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2827,11 +2722,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W1304"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="M389" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29:Q397"/>
+      <selection pane="bottomRight" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2846,48 +2741,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="11"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="8"/>
     </row>
     <row r="3" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2962,7 +2857,7 @@
         <v>29</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>30</v>
@@ -3049,1017 +2944,387 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2022</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B6"/>
+      <c r="D6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
       <c r="I6"/>
-      <c r="K6">
-        <v>1000000</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
       <c r="P6"/>
-      <c r="Q6" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="Q6"/>
       <c r="R6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2022</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B7"/>
+      <c r="D7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
       <c r="I7"/>
-      <c r="J7">
-        <v>1000000</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
       <c r="R7" s="1"/>
       <c r="T7" s="1"/>
       <c r="W7" s="1"/>
     </row>
     <row r="8" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>2022</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B8"/>
+      <c r="D8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
       <c r="I8"/>
-      <c r="K8">
-        <v>768000</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>69</v>
-      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
       <c r="R8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>2022</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B9"/>
+      <c r="D9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
       <c r="I9"/>
-      <c r="J9">
-        <v>768000</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
       <c r="P9"/>
+      <c r="Q9"/>
       <c r="R9" s="1"/>
       <c r="T9" s="1"/>
       <c r="W9" s="1"/>
     </row>
     <row r="10" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>2023</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B10"/>
+      <c r="D10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
       <c r="I10"/>
-      <c r="K10">
-        <v>1000000</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
       <c r="P10"/>
-      <c r="Q10" t="s">
-        <v>67</v>
-      </c>
+      <c r="Q10"/>
       <c r="R10" s="1"/>
       <c r="T10" s="1"/>
       <c r="W10" s="1"/>
     </row>
     <row r="11" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>2023</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B11"/>
+      <c r="D11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
       <c r="I11"/>
-      <c r="J11">
-        <v>1000000</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
       <c r="P11"/>
+      <c r="Q11"/>
       <c r="R11" s="1"/>
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>2023</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B12"/>
+      <c r="D12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
       <c r="I12"/>
-      <c r="K12">
-        <v>500000</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
       <c r="P12"/>
-      <c r="Q12" t="s">
-        <v>67</v>
-      </c>
+      <c r="Q12"/>
       <c r="R12" s="1"/>
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>2023</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B13"/>
+      <c r="D13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
       <c r="I13"/>
-      <c r="J13">
-        <v>500000</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
       <c r="P13"/>
+      <c r="Q13"/>
       <c r="R13" s="1"/>
       <c r="T13" s="1"/>
       <c r="W13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>2023</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B14"/>
+      <c r="D14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
       <c r="I14"/>
-      <c r="K14">
-        <v>200000</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
       <c r="P14"/>
-      <c r="Q14" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="Q14"/>
       <c r="R14" s="1"/>
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>2023</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B15"/>
+      <c r="D15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
       <c r="I15"/>
-      <c r="K15">
-        <v>200000</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
       <c r="P15"/>
-      <c r="Q15" t="s">
-        <v>71</v>
-      </c>
+      <c r="Q15"/>
       <c r="R15" s="1"/>
       <c r="T15" s="1"/>
       <c r="W15" s="1"/>
     </row>
     <row r="16" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <v>2023</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B16"/>
+      <c r="D16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
       <c r="I16"/>
-      <c r="J16">
-        <v>400000</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
       <c r="P16"/>
+      <c r="Q16"/>
       <c r="R16" s="1"/>
       <c r="T16" s="1"/>
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>2023</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B17"/>
+      <c r="D17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
       <c r="I17"/>
-      <c r="K17">
-        <v>2200000</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
       <c r="P17"/>
-      <c r="Q17" t="s">
-        <v>69</v>
-      </c>
+      <c r="Q17"/>
       <c r="R17" s="1"/>
       <c r="T17" s="1"/>
       <c r="W17" s="1"/>
     </row>
     <row r="18" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <v>6</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>2023</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B18"/>
+      <c r="D18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
       <c r="I18"/>
-      <c r="J18">
-        <v>2200000</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
       <c r="R18" s="1"/>
       <c r="T18" s="1"/>
       <c r="W18" s="1"/>
     </row>
     <row r="19" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>2023</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B19"/>
+      <c r="D19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
       <c r="I19"/>
-      <c r="K19">
-        <v>5000000</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
       <c r="R19" s="1"/>
       <c r="T19" s="1"/>
       <c r="W19" s="1"/>
     </row>
     <row r="20" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>2023</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B20"/>
+      <c r="D20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
       <c r="I20"/>
-      <c r="J20">
-        <v>5000000</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
       <c r="Q20"/>
       <c r="R20" s="1"/>
       <c r="T20" s="1"/>
     </row>
     <row r="21" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <v>8</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>2023</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B21"/>
+      <c r="D21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
       <c r="I21"/>
-      <c r="K21">
-        <v>750000</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
       <c r="P21"/>
-      <c r="Q21" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="Q21"/>
       <c r="R21" s="1"/>
       <c r="T21" s="1"/>
     </row>
     <row r="22" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <v>8</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22">
-        <v>2023</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B22"/>
+      <c r="D22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
       <c r="I22"/>
-      <c r="J22">
-        <v>750000</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
       <c r="P22"/>
+      <c r="Q22"/>
       <c r="R22" s="1"/>
       <c r="T22" s="1"/>
       <c r="W22" s="1"/>
     </row>
     <row r="23" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23">
-        <v>9</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>2023</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B23"/>
+      <c r="D23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
       <c r="I23"/>
-      <c r="K23">
-        <v>2900000</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
       <c r="P23"/>
-      <c r="Q23" t="s">
-        <v>69</v>
-      </c>
+      <c r="Q23"/>
       <c r="R23" s="1"/>
       <c r="T23" s="1"/>
     </row>
     <row r="24" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24">
-        <v>9</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24">
-        <v>2023</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B24"/>
+      <c r="D24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
       <c r="I24"/>
-      <c r="J24">
-        <v>2900000</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
       <c r="P24"/>
+      <c r="Q24"/>
       <c r="R24" s="1"/>
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <v>10</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>2021</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B25"/>
+      <c r="D25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
       <c r="I25"/>
-      <c r="K25">
-        <v>2000000</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
       <c r="P25"/>
-      <c r="Q25" t="s">
-        <v>69</v>
-      </c>
+      <c r="Q25"/>
       <c r="R25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
     <row r="26" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26">
-        <v>10</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <v>2021</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B26"/>
+      <c r="D26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
       <c r="I26"/>
-      <c r="J26">
-        <v>2000000</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
       <c r="P26"/>
+      <c r="Q26"/>
       <c r="R26" s="1"/>
       <c r="T26" s="1"/>
       <c r="W26" s="1"/>
     </row>
     <row r="27" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27">
-        <v>11</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>2023</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B27"/>
+      <c r="D27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
       <c r="I27"/>
-      <c r="K27">
-        <v>70000</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
       <c r="P27"/>
-      <c r="Q27" t="s">
-        <v>67</v>
-      </c>
+      <c r="Q27"/>
       <c r="R27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="W27" s="1"/>
     </row>
     <row r="28" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28">
-        <v>11</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28">
-        <v>2023</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B28"/>
+      <c r="D28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
       <c r="I28"/>
-      <c r="J28">
-        <v>70000</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
       <c r="P28"/>
+      <c r="Q28"/>
       <c r="R28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
@@ -4067,7 +3332,16 @@
     <row r="29" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29"/>
       <c r="D29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
       <c r="I29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
       <c r="R29" s="1"/>
       <c r="T29" s="1"/>
       <c r="W29" s="1"/>
@@ -4075,7 +3349,15 @@
     <row r="30" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30"/>
       <c r="D30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
       <c r="I30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
       <c r="Q30"/>
       <c r="R30" s="1"/>
       <c r="T30" s="1"/>
@@ -4084,15 +3366,30 @@
     <row r="31" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31"/>
       <c r="D31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
       <c r="I31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
       <c r="P31"/>
+      <c r="Q31"/>
       <c r="R31" s="1"/>
       <c r="T31" s="1"/>
     </row>
     <row r="32" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32"/>
       <c r="D32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
       <c r="I32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
       <c r="P32"/>
       <c r="Q32"/>
       <c r="R32" s="1"/>
@@ -4102,8 +3399,16 @@
     <row r="33" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33"/>
       <c r="D33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
       <c r="I33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
       <c r="P33"/>
+      <c r="Q33"/>
       <c r="R33" s="1"/>
       <c r="T33" s="1"/>
       <c r="W33" s="1"/>
@@ -4111,7 +3416,14 @@
     <row r="34" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34"/>
       <c r="D34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
       <c r="I34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
       <c r="P34"/>
       <c r="Q34"/>
       <c r="R34" s="1"/>
@@ -4120,8 +3432,16 @@
     <row r="35" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35"/>
       <c r="D35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
       <c r="I35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
       <c r="P35"/>
+      <c r="Q35"/>
       <c r="R35" s="1"/>
       <c r="T35" s="1"/>
       <c r="W35" s="1"/>
@@ -4129,8 +3449,16 @@
     <row r="36" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36"/>
       <c r="D36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
       <c r="I36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
       <c r="P36"/>
+      <c r="Q36"/>
       <c r="R36" s="1"/>
       <c r="T36" s="1"/>
       <c r="W36" s="1"/>
@@ -4138,7 +3466,14 @@
     <row r="37" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37"/>
       <c r="D37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
       <c r="I37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
       <c r="P37"/>
       <c r="Q37"/>
       <c r="R37" s="1"/>
@@ -4147,8 +3482,16 @@
     <row r="38" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38"/>
       <c r="D38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
       <c r="I38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
       <c r="P38"/>
+      <c r="Q38"/>
       <c r="R38" s="1"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
@@ -4157,8 +3500,14 @@
     <row r="39" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39"/>
       <c r="D39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
       <c r="I39"/>
-      <c r="K39" s="7"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
       <c r="P39"/>
       <c r="Q39"/>
       <c r="R39" s="1"/>
@@ -4168,29 +3517,33 @@
     <row r="40" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40"/>
       <c r="D40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
       <c r="I40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
       <c r="P40"/>
+      <c r="Q40"/>
       <c r="R40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
     </row>
     <row r="41" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
+      <c r="B41"/>
+      <c r="D41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
       <c r="R41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
@@ -4198,8 +3551,16 @@
     <row r="42" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42"/>
       <c r="D42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
       <c r="I42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
       <c r="P42"/>
+      <c r="Q42"/>
       <c r="R42" s="1"/>
       <c r="T42" s="1"/>
       <c r="W42" s="1"/>
@@ -4207,7 +3568,14 @@
     <row r="43" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43"/>
       <c r="D43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
       <c r="I43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
       <c r="P43"/>
       <c r="Q43"/>
       <c r="R43" s="1"/>

</xml_diff>